<commit_message>
added : about functionality tab, changed : make tab body max height dynamic and always apply
</commit_message>
<xml_diff>
--- a/data/db_source/__meta_schema__.xlsx
+++ b/data/db_source/__meta_schema__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689C9828-6427-FA48-8433-DACF502CA567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4638EFDA-B734-1943-A292-852528CDDEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2680" yWindow="500" windowWidth="26120" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="189">
   <si>
     <t>id</t>
   </si>
@@ -561,16 +561,64 @@
   </si>
   <si>
     <t>Variables contenues dans les datasets</t>
+  </si>
+  <si>
+    <t>tag_ids</t>
+  </si>
+  <si>
+    <t>doc_ids</t>
+  </si>
+  <si>
+    <t>last_update</t>
+  </si>
+  <si>
+    <t>timestamp unix de la dernière modification</t>
+  </si>
+  <si>
+    <t>clés des docs liés</t>
+  </si>
+  <si>
+    <t>clés des mots clés liés</t>
+  </si>
+  <si>
+    <t>clé du mot clé parent</t>
+  </si>
+  <si>
+    <t>original_name</t>
+  </si>
+  <si>
+    <t>modality_ids</t>
+  </si>
+  <si>
+    <t>nom d'origine de la variable</t>
+  </si>
+  <si>
+    <t>début de la période couverte par la variable</t>
+  </si>
+  <si>
+    <t>fin de la période couverte par la variable</t>
+  </si>
+  <si>
+    <t>clé des modalités liées</t>
+  </si>
+  <si>
+    <t>timestamp unix de l'ajout du favori</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -596,8 +644,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,10 +665,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CC52189E-6718-7640-A09D-3E13A3AE1ED2}" name="Tableau3" displayName="Tableau3" ref="A1:D120" totalsRowShown="0">
-  <autoFilter ref="A1:D120" xr:uid="{CC52189E-6718-7640-A09D-3E13A3AE1ED2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D120">
-    <sortCondition ref="A1:A120"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CC52189E-6718-7640-A09D-3E13A3AE1ED2}" name="Tableau3" displayName="Tableau3" ref="A1:D134" totalsRowShown="0">
+  <autoFilter ref="A1:D134" xr:uid="{CC52189E-6718-7640-A09D-3E13A3AE1ED2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D134">
+    <sortCondition ref="A1:A134"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="4" xr3:uid="{D4AE5F0B-EFF7-F144-B9F0-6F582D88D1B3}" name="folder"/>
@@ -953,11 +1002,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D120"/>
+  <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1336,10 +1385,13 @@
         <v>152</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>175</v>
       </c>
       <c r="D28" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1347,13 +1399,13 @@
         <v>152</v>
       </c>
       <c r="B29" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>176</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1363,11 +1415,8 @@
       <c r="B30" t="s">
         <v>110</v>
       </c>
-      <c r="C30" t="s">
-        <v>83</v>
-      </c>
       <c r="D30" t="s">
-        <v>126</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1378,10 +1427,10 @@
         <v>110</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1392,10 +1441,10 @@
         <v>110</v>
       </c>
       <c r="C32" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="D32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1406,10 +1455,10 @@
         <v>110</v>
       </c>
       <c r="C33" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1420,10 +1469,10 @@
         <v>110</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1434,10 +1483,10 @@
         <v>110</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="D35" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1448,10 +1497,10 @@
         <v>110</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1459,10 +1508,13 @@
         <v>152</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>110</v>
+      </c>
+      <c r="C37" t="s">
+        <v>111</v>
       </c>
       <c r="D37" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1470,13 +1522,13 @@
         <v>152</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C38" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1484,13 +1536,13 @@
         <v>152</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
+        <v>177</v>
       </c>
       <c r="D39" t="s">
-        <v>131</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1498,10 +1550,10 @@
         <v>152</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>112</v>
       </c>
       <c r="D40" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1509,13 +1561,13 @@
         <v>152</v>
       </c>
       <c r="B41" t="s">
-        <v>26</v>
+        <v>112</v>
       </c>
       <c r="C41" t="s">
-        <v>142</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1523,13 +1575,13 @@
         <v>152</v>
       </c>
       <c r="B42" t="s">
-        <v>26</v>
+        <v>112</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1539,11 +1591,8 @@
       <c r="B43" t="s">
         <v>26</v>
       </c>
-      <c r="C43" t="s">
-        <v>1</v>
-      </c>
       <c r="D43" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1554,10 +1603,10 @@
         <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="D44" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1568,10 +1617,10 @@
         <v>26</v>
       </c>
       <c r="C45" t="s">
-        <v>145</v>
+        <v>102</v>
       </c>
       <c r="D45" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1582,10 +1631,10 @@
         <v>26</v>
       </c>
       <c r="C46" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1596,10 +1645,10 @@
         <v>26</v>
       </c>
       <c r="C47" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="D47" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1610,10 +1659,10 @@
         <v>26</v>
       </c>
       <c r="C48" t="s">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="D48" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1624,10 +1673,10 @@
         <v>26</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1638,10 +1687,10 @@
         <v>26</v>
       </c>
       <c r="C50" t="s">
-        <v>144</v>
+        <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1652,10 +1701,10 @@
         <v>26</v>
       </c>
       <c r="C51" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="D51" t="s">
-        <v>46</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1666,10 +1715,10 @@
         <v>26</v>
       </c>
       <c r="C52" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D52" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1680,10 +1729,10 @@
         <v>26</v>
       </c>
       <c r="C53" t="s">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="D53" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1694,10 +1743,10 @@
         <v>26</v>
       </c>
       <c r="C54" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D54" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1708,10 +1757,10 @@
         <v>26</v>
       </c>
       <c r="C55" t="s">
-        <v>135</v>
+        <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1722,10 +1771,10 @@
         <v>26</v>
       </c>
       <c r="C56" t="s">
-        <v>101</v>
+        <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1736,10 +1785,10 @@
         <v>26</v>
       </c>
       <c r="C57" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D57" t="s">
-        <v>147</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1747,10 +1796,13 @@
         <v>152</v>
       </c>
       <c r="B58" t="s">
-        <v>113</v>
+        <v>26</v>
+      </c>
+      <c r="C58" t="s">
+        <v>135</v>
       </c>
       <c r="D58" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1758,13 +1810,13 @@
         <v>152</v>
       </c>
       <c r="B59" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="C59" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="D59" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1772,13 +1824,13 @@
         <v>152</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="C60" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D60" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1786,10 +1838,13 @@
         <v>152</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>26</v>
+      </c>
+      <c r="C61" t="s">
+        <v>175</v>
       </c>
       <c r="D61" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1797,13 +1852,13 @@
         <v>152</v>
       </c>
       <c r="B62" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
       <c r="C62" t="s">
-        <v>1</v>
+        <v>176</v>
       </c>
       <c r="D62" t="s">
-        <v>6</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -1811,13 +1866,10 @@
         <v>152</v>
       </c>
       <c r="B63" t="s">
-        <v>95</v>
-      </c>
-      <c r="C63" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="D63" t="s">
-        <v>99</v>
+        <v>164</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1825,13 +1877,13 @@
         <v>152</v>
       </c>
       <c r="B64" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="C64" t="s">
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>54</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1839,13 +1891,13 @@
         <v>152</v>
       </c>
       <c r="B65" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="C65" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D65" t="s">
-        <v>5</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -1855,11 +1907,8 @@
       <c r="B66" t="s">
         <v>95</v>
       </c>
-      <c r="C66" t="s">
-        <v>3</v>
-      </c>
       <c r="D66" t="s">
-        <v>70</v>
+        <v>165</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -1870,10 +1919,10 @@
         <v>95</v>
       </c>
       <c r="C67" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -1884,10 +1933,10 @@
         <v>95</v>
       </c>
       <c r="C68" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D68" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -1895,10 +1944,13 @@
         <v>152</v>
       </c>
       <c r="B69" t="s">
-        <v>28</v>
+        <v>95</v>
+      </c>
+      <c r="C69" t="s">
+        <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>167</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -1906,13 +1958,13 @@
         <v>152</v>
       </c>
       <c r="B70" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="C70" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D70" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -1920,13 +1972,13 @@
         <v>152</v>
       </c>
       <c r="B71" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="C71" t="s">
-        <v>96</v>
+        <v>3</v>
       </c>
       <c r="D71" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -1934,10 +1986,13 @@
         <v>152</v>
       </c>
       <c r="B72" t="s">
-        <v>71</v>
+        <v>95</v>
+      </c>
+      <c r="C72" t="s">
+        <v>14</v>
       </c>
       <c r="D72" t="s">
-        <v>168</v>
+        <v>49</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1945,13 +2000,13 @@
         <v>152</v>
       </c>
       <c r="B73" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="C73" t="s">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="D73" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -1959,13 +2014,13 @@
         <v>152</v>
       </c>
       <c r="B74" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="C74" t="s">
-        <v>9</v>
+        <v>175</v>
       </c>
       <c r="D74" t="s">
-        <v>114</v>
+        <v>180</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -1973,13 +2028,13 @@
         <v>152</v>
       </c>
       <c r="B75" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="C75" t="s">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="D75" t="s">
-        <v>74</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -1987,13 +2042,10 @@
         <v>152</v>
       </c>
       <c r="B76" t="s">
-        <v>71</v>
-      </c>
-      <c r="C76" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D76" t="s">
-        <v>73</v>
+        <v>167</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2001,13 +2053,13 @@
         <v>152</v>
       </c>
       <c r="B77" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="C77" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2015,10 +2067,13 @@
         <v>152</v>
       </c>
       <c r="B78" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="C78" t="s">
+        <v>96</v>
       </c>
       <c r="D78" t="s">
-        <v>170</v>
+        <v>67</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2026,13 +2081,10 @@
         <v>152</v>
       </c>
       <c r="B79" t="s">
-        <v>27</v>
-      </c>
-      <c r="C79" t="s">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="D79" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2040,13 +2092,13 @@
         <v>152</v>
       </c>
       <c r="B80" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="C80" t="s">
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -2054,10 +2106,13 @@
         <v>152</v>
       </c>
       <c r="B81" t="s">
-        <v>19</v>
+        <v>71</v>
+      </c>
+      <c r="C81" t="s">
+        <v>9</v>
       </c>
       <c r="D81" t="s">
-        <v>172</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -2065,13 +2120,13 @@
         <v>152</v>
       </c>
       <c r="B82" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C82" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -2079,13 +2134,13 @@
         <v>152</v>
       </c>
       <c r="B83" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C83" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D83" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -2093,13 +2148,13 @@
         <v>152</v>
       </c>
       <c r="B84" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C84" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D84" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -2107,10 +2162,10 @@
         <v>152</v>
       </c>
       <c r="B85" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D85" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -2118,13 +2173,13 @@
         <v>152</v>
       </c>
       <c r="B86" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C86" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -2132,13 +2187,13 @@
         <v>152</v>
       </c>
       <c r="B87" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C87" t="s">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="D87" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -2146,13 +2201,10 @@
         <v>152</v>
       </c>
       <c r="B88" t="s">
-        <v>20</v>
-      </c>
-      <c r="C88" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="D88" t="s">
-        <v>53</v>
+        <v>172</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -2160,13 +2212,13 @@
         <v>152</v>
       </c>
       <c r="B89" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C89" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D89" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -2174,10 +2226,13 @@
         <v>152</v>
       </c>
       <c r="B90" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="C90" t="s">
+        <v>0</v>
       </c>
       <c r="D90" t="s">
-        <v>174</v>
+        <v>57</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -2185,13 +2240,13 @@
         <v>152</v>
       </c>
       <c r="B91" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C91" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D91" t="s">
-        <v>65</v>
+        <v>181</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -2199,13 +2254,13 @@
         <v>152</v>
       </c>
       <c r="B92" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C92" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D92" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -2213,13 +2268,10 @@
         <v>152</v>
       </c>
       <c r="B93" t="s">
-        <v>21</v>
-      </c>
-      <c r="C93" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D93" t="s">
-        <v>58</v>
+        <v>173</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -2227,13 +2279,13 @@
         <v>152</v>
       </c>
       <c r="B94" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C94" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D94" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -2241,13 +2293,13 @@
         <v>152</v>
       </c>
       <c r="B95" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C95" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D95" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -2255,13 +2307,13 @@
         <v>152</v>
       </c>
       <c r="B96" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C96" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="D96" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -2269,13 +2321,13 @@
         <v>152</v>
       </c>
       <c r="B97" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C97" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D97" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -2285,192 +2337,198 @@
       <c r="B98" t="s">
         <v>21</v>
       </c>
-      <c r="C98" t="s">
-        <v>7</v>
-      </c>
       <c r="D98" t="s">
-        <v>77</v>
+        <v>174</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>154</v>
+        <v>152</v>
+      </c>
+      <c r="B99" t="s">
+        <v>21</v>
+      </c>
+      <c r="C99" t="s">
+        <v>2</v>
       </c>
       <c r="D99" t="s">
-        <v>155</v>
+        <v>65</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B100" t="s">
-        <v>81</v>
+        <v>21</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>160</v>
+        <v>44</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B101" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="C101" t="s">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="D101" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B102" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="C102" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="D102" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B103" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="C103" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D103" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B104" t="s">
-        <v>115</v>
+        <v>21</v>
+      </c>
+      <c r="C104" t="s">
+        <v>23</v>
       </c>
       <c r="D104" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B105" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="C105" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D105" t="s">
-        <v>130</v>
+        <v>43</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B106" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="C106" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
       <c r="D106" t="s">
-        <v>132</v>
+        <v>77</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B107" t="s">
-        <v>86</v>
+        <v>21</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="D107" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B108" t="s">
-        <v>86</v>
-      </c>
-      <c r="C108" t="s">
-        <v>88</v>
+        <v>21</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="D108" t="s">
-        <v>89</v>
+        <v>185</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B109" t="s">
-        <v>86</v>
-      </c>
-      <c r="C109" t="s">
-        <v>83</v>
+        <v>21</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="D109" t="s">
-        <v>90</v>
+        <v>186</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B110" t="s">
-        <v>86</v>
-      </c>
-      <c r="C110" t="s">
-        <v>84</v>
+        <v>21</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="D110" t="s">
-        <v>91</v>
+        <v>187</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B111" t="s">
-        <v>86</v>
-      </c>
-      <c r="C111" t="s">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="D111" t="s">
-        <v>87</v>
+        <v>180</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>154</v>
       </c>
-      <c r="B112" t="s">
-        <v>86</v>
-      </c>
-      <c r="C112" t="s">
-        <v>93</v>
-      </c>
       <c r="D112" t="s">
-        <v>94</v>
+        <v>155</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -2478,10 +2536,10 @@
         <v>154</v>
       </c>
       <c r="B113" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D113" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -2489,13 +2547,13 @@
         <v>154</v>
       </c>
       <c r="B114" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C114" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="D114" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -2503,13 +2561,13 @@
         <v>154</v>
       </c>
       <c r="B115" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C115" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="D115" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -2517,10 +2575,13 @@
         <v>154</v>
       </c>
       <c r="B116" t="s">
-        <v>117</v>
+        <v>81</v>
+      </c>
+      <c r="C116" t="s">
+        <v>0</v>
       </c>
       <c r="D116" t="s">
-        <v>171</v>
+        <v>82</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -2528,13 +2589,13 @@
         <v>154</v>
       </c>
       <c r="B117" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="C117" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="D117" t="s">
-        <v>121</v>
+        <v>188</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -2542,13 +2603,10 @@
         <v>154</v>
       </c>
       <c r="B118" t="s">
-        <v>117</v>
-      </c>
-      <c r="C118" t="s">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="D118" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -2556,13 +2614,13 @@
         <v>154</v>
       </c>
       <c r="B119" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C119" t="s">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="D119" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -2570,16 +2628,204 @@
         <v>154</v>
       </c>
       <c r="B120" t="s">
+        <v>115</v>
+      </c>
+      <c r="C120" t="s">
+        <v>116</v>
+      </c>
+      <c r="D120" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>154</v>
+      </c>
+      <c r="B121" t="s">
+        <v>86</v>
+      </c>
+      <c r="D121" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>154</v>
+      </c>
+      <c r="B122" t="s">
+        <v>86</v>
+      </c>
+      <c r="C122" t="s">
+        <v>88</v>
+      </c>
+      <c r="D122" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>154</v>
+      </c>
+      <c r="B123" t="s">
+        <v>86</v>
+      </c>
+      <c r="C123" t="s">
+        <v>83</v>
+      </c>
+      <c r="D123" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>154</v>
+      </c>
+      <c r="B124" t="s">
+        <v>86</v>
+      </c>
+      <c r="C124" t="s">
+        <v>84</v>
+      </c>
+      <c r="D124" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>154</v>
+      </c>
+      <c r="B125" t="s">
+        <v>86</v>
+      </c>
+      <c r="C125" t="s">
+        <v>0</v>
+      </c>
+      <c r="D125" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>154</v>
+      </c>
+      <c r="B126" t="s">
+        <v>86</v>
+      </c>
+      <c r="C126" t="s">
+        <v>93</v>
+      </c>
+      <c r="D126" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>154</v>
+      </c>
+      <c r="B127" t="s">
+        <v>78</v>
+      </c>
+      <c r="D127" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>154</v>
+      </c>
+      <c r="B128" t="s">
+        <v>78</v>
+      </c>
+      <c r="C128" t="s">
+        <v>0</v>
+      </c>
+      <c r="D128" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>154</v>
+      </c>
+      <c r="B129" t="s">
+        <v>78</v>
+      </c>
+      <c r="C129" t="s">
+        <v>20</v>
+      </c>
+      <c r="D129" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>154</v>
+      </c>
+      <c r="B130" t="s">
         <v>117</v>
       </c>
-      <c r="C120" t="s">
+      <c r="D130" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>154</v>
+      </c>
+      <c r="B131" t="s">
+        <v>117</v>
+      </c>
+      <c r="C131" t="s">
+        <v>118</v>
+      </c>
+      <c r="D131" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>154</v>
+      </c>
+      <c r="B132" t="s">
+        <v>117</v>
+      </c>
+      <c r="C132" t="s">
+        <v>0</v>
+      </c>
+      <c r="D132" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>154</v>
+      </c>
+      <c r="B133" t="s">
+        <v>117</v>
+      </c>
+      <c r="C133" t="s">
+        <v>119</v>
+      </c>
+      <c r="D133" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>154</v>
+      </c>
+      <c r="B134" t="s">
+        <v>117</v>
+      </c>
+      <c r="C134" t="s">
         <v>93</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D134" t="s">
         <v>123</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>